<commit_message>
Created TruckRoutes for figuring out truck routes
</commit_message>
<xml_diff>
--- a/data/package_details.xlsx
+++ b/data/package_details.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dustinwurtz/Documents/wgu/c950/final_project/deliver_mapping/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFAA238A-7C0E-7149-956C-1643655FF531}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56B77164-73E6-C24C-A0B4-E607262D4227}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-38400" yWindow="880" windowWidth="38400" windowHeight="21600" xr2:uid="{AA7E8E45-A839-A841-A8EA-D36605D0FCA2}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="44">
   <si>
     <t>EOD</t>
   </si>
@@ -47,10 +47,7 @@
     <t>233 Canyon Rd</t>
   </si>
   <si>
-    <t>Truck 1 - Mostly Priority</t>
-  </si>
-  <si>
-    <t>Truck 2 - Mostly EOD</t>
+    <t>Truck 1</t>
   </si>
   <si>
     <t>Package</t>
@@ -62,9 +59,6 @@
     <t>Special Notes</t>
   </si>
   <si>
-    <t>Only on Truck 2</t>
-  </si>
-  <si>
     <t>380 W 2880 S</t>
   </si>
   <si>
@@ -77,20 +71,110 @@
     <t>3060 Lester St</t>
   </si>
   <si>
-    <t>Won't arrive till 9:05</t>
-  </si>
-  <si>
     <t>1330 2100 S</t>
   </si>
   <si>
     <t>300 State St</t>
+  </si>
+  <si>
+    <t>Truck 2 - Leaves Later</t>
+  </si>
+  <si>
+    <t>Truck 3 - Actually Truck 1</t>
+  </si>
+  <si>
+    <t>Can only be on truck 2</t>
+  </si>
+  <si>
+    <t>Delayed on flight---will not arrive to depot until 9:05 am</t>
+  </si>
+  <si>
+    <t>Wrong address listed</t>
+  </si>
+  <si>
+    <t>Must be delivered with 15, 19</t>
+  </si>
+  <si>
+    <t>Must be delivered with 13, 19</t>
+  </si>
+  <si>
+    <t>Must be delivered with 13, 15</t>
+  </si>
+  <si>
+    <t>Address</t>
+  </si>
+  <si>
+    <t>600 E 900 South</t>
+  </si>
+  <si>
+    <t>2600 Taylorsville Blvd</t>
+  </si>
+  <si>
+    <t>3575 W Valley Central Station bus Loop</t>
+  </si>
+  <si>
+    <t>2010 W 500 S</t>
+  </si>
+  <si>
+    <t>4300 S 1300 E</t>
+  </si>
+  <si>
+    <t>4580 S 2300 E</t>
+  </si>
+  <si>
+    <t>3148 S 1100 W</t>
+  </si>
+  <si>
+    <t>1488 4800 S</t>
+  </si>
+  <si>
+    <t>177 W Price Ave</t>
+  </si>
+  <si>
+    <t>3595 Main St</t>
+  </si>
+  <si>
+    <t>6351 South 900 East</t>
+  </si>
+  <si>
+    <t>5100 South 2700 West</t>
+  </si>
+  <si>
+    <t>5025 State St</t>
+  </si>
+  <si>
+    <t>1060 Dalton Ave S</t>
+  </si>
+  <si>
+    <t>2835 Main St</t>
+  </si>
+  <si>
+    <t>3365 S 900 W</t>
+  </si>
+  <si>
+    <t>2300 Parkway Blvd</t>
+  </si>
+  <si>
+    <t>5383 S 900 East #104</t>
+  </si>
+  <si>
+    <t>When at a deliver stop, check for a duplicate address on another package</t>
+  </si>
+  <si>
+    <t>Duplicate address due at EOD</t>
+  </si>
+  <si>
+    <t>Priority, needs to be delivered before 9:00am or 10:30am</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="[$-409]h:mm\ AM/PM;@"/>
+  </numFmts>
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -98,13 +182,31 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -119,9 +221,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -436,136 +546,567 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD25CE7E-4589-6D4B-B4AF-BCA39781F14E}">
-  <dimension ref="A1:I9"/>
+  <dimension ref="A1:J41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="J20" sqref="J20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="7.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.1640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="27" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="27.6640625" customWidth="1"/>
+    <col min="1" max="1" width="7.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="34" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="48.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="10.83203125" style="1"/>
+    <col min="10" max="10" width="62.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="27.6640625" style="1" customWidth="1"/>
+    <col min="12" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C1" t="s">
+      <c r="J1" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2">
+        <v>0.4375</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="G2" s="3"/>
+      <c r="J2" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A3" s="1">
+        <v>2</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G3" s="3"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A4" s="1">
+        <v>3</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A5" s="1">
         <v>4</v>
       </c>
-      <c r="D1" t="s">
+      <c r="B5" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G5" s="3"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A6" s="1">
         <v>5</v>
       </c>
-      <c r="E1" t="s">
+      <c r="B6" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G6" s="3"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A7" s="1">
+        <v>6</v>
+      </c>
+      <c r="B7" s="2">
+        <v>0.4375</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A8" s="1">
+        <v>7</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G8" s="3"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A9" s="1">
         <v>8</v>
       </c>
-      <c r="I1" t="s">
+      <c r="B9" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G9" s="3"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A10" s="1">
+        <v>9</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A11" s="1">
+        <v>10</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="G11" s="3"/>
+      <c r="I11" s="7"/>
+      <c r="J11" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A12" s="1">
+        <v>11</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="G12" s="3"/>
+      <c r="I12" s="5"/>
+      <c r="J12" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A13" s="1">
         <v>12</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" s="1">
-        <v>0.4375</v>
-      </c>
-      <c r="C2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A3">
+      <c r="B13" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="G13" s="3"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A14" s="1">
+        <v>13</v>
+      </c>
+      <c r="B14" s="2">
+        <v>0.4375</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="G14" s="3"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A15" s="1">
+        <v>14</v>
+      </c>
+      <c r="B15" s="2">
+        <v>0.4375</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="G15" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A16" s="1">
+        <v>15</v>
+      </c>
+      <c r="B16" s="2">
+        <v>0.375</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="G16" s="3"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A17" s="1">
+        <v>16</v>
+      </c>
+      <c r="B17" s="2">
+        <v>0.4375</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="G17" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A18" s="1">
+        <v>17</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="G18" s="3"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A19" s="1">
+        <v>18</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="G19" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A20" s="1">
+        <v>19</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="G20" s="3"/>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A21" s="1">
+        <v>20</v>
+      </c>
+      <c r="B21" s="2">
+        <v>0.4375</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="G21" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A22" s="1">
+        <v>21</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D22" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="G22" s="3"/>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A23" s="1">
+        <v>22</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="G23" s="3"/>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A24" s="1">
+        <v>23</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="G24" s="3"/>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A25" s="1">
+        <v>24</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="G25" s="3"/>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A26" s="1">
+        <v>25</v>
+      </c>
+      <c r="B26" s="2">
+        <v>0.4375</v>
+      </c>
+      <c r="E26" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="G26" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A27" s="1">
+        <v>26</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E27" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="G27" s="3"/>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A28" s="1">
+        <v>27</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="G28" s="3"/>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A29" s="1">
+        <v>28</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E29" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="G29" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A30" s="1">
+        <v>29</v>
+      </c>
+      <c r="B30" s="2">
+        <v>0.4375</v>
+      </c>
+      <c r="D30" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G30" s="3"/>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A31" s="1">
+        <v>30</v>
+      </c>
+      <c r="B31" s="2">
+        <v>0.4375</v>
+      </c>
+      <c r="D31" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G31" s="3"/>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A32" s="1">
+        <v>31</v>
+      </c>
+      <c r="B32" s="2">
+        <v>0.4375</v>
+      </c>
+      <c r="E32" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="G32" s="3"/>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A33" s="1">
+        <v>32</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E33" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="G33" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A34" s="1">
+        <v>33</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C34" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
-        <v>0</v>
-      </c>
-      <c r="D3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>0</v>
-      </c>
-      <c r="D4" t="s">
-        <v>3</v>
-      </c>
-      <c r="E4" t="s">
+      <c r="G34" s="3"/>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A35" s="1">
+        <v>34</v>
+      </c>
+      <c r="B35" s="2">
+        <v>0.4375</v>
+      </c>
+      <c r="D35" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="G35" s="3"/>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A36" s="1">
+        <v>35</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C36" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="G36" s="3"/>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A37" s="1">
+        <v>36</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E37" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="G37" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A38" s="1">
+        <v>37</v>
+      </c>
+      <c r="B38" s="2">
+        <v>0.4375</v>
+      </c>
+      <c r="E38" s="4" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
-        <v>0</v>
-      </c>
-      <c r="D5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A6">
-        <v>5</v>
-      </c>
-      <c r="B6" t="s">
-        <v>0</v>
-      </c>
-      <c r="D6" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A7">
-        <v>6</v>
-      </c>
-      <c r="B7" s="1">
-        <v>0.4375</v>
-      </c>
-      <c r="D7" t="s">
-        <v>13</v>
-      </c>
-      <c r="E7" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A8">
-        <v>7</v>
-      </c>
-      <c r="B8" t="s">
-        <v>0</v>
-      </c>
-      <c r="D8" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A9">
+      <c r="G38" s="3"/>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A39" s="1">
+        <v>38</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E39" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="G39" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A40" s="1">
+        <v>39</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C40" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="G40" s="3"/>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A41" s="1">
+        <v>40</v>
+      </c>
+      <c r="B41" s="2">
+        <v>0.4375</v>
+      </c>
+      <c r="D41" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B9" t="s">
-        <v>0</v>
-      </c>
-      <c r="D9" t="s">
-        <v>16</v>
-      </c>
+      <c r="G41" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Completed first trucks deliver of priority packages
</commit_message>
<xml_diff>
--- a/data/package_details.xlsx
+++ b/data/package_details.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dustinwurtz/Documents/wgu/c950/final_project/deliver_mapping/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56B77164-73E6-C24C-A0B4-E607262D4227}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8A3DFDC-E5EF-D242-B8D9-4FD9250A09B2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38400" yWindow="880" windowWidth="38400" windowHeight="21600" xr2:uid="{AA7E8E45-A839-A841-A8EA-D36605D0FCA2}"/>
+    <workbookView xWindow="-76800" yWindow="880" windowWidth="38400" windowHeight="21600" xr2:uid="{AA7E8E45-A839-A841-A8EA-D36605D0FCA2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="45">
   <si>
     <t>EOD</t>
   </si>
@@ -165,6 +165,9 @@
   </si>
   <si>
     <t>Priority, needs to be delivered before 9:00am or 10:30am</t>
+  </si>
+  <si>
+    <t>410 S State St (Was 300 State)</t>
   </si>
 </sst>
 </file>
@@ -549,7 +552,7 @@
   <dimension ref="A1:J41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J20" sqref="J20"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -559,7 +562,7 @@
     <col min="3" max="3" width="34" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="17.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="19" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="21.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="27" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="48.1640625" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="9" width="10.83203125" style="1"/>
     <col min="10" max="10" width="62.33203125" style="1" bestFit="1" customWidth="1"/>
@@ -653,7 +656,8 @@
       <c r="B6" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="3"/>
+      <c r="F6" s="6" t="s">
         <v>9</v>
       </c>
       <c r="G6" s="3"/>
@@ -691,7 +695,7 @@
       <c r="B9" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="F9" s="3" t="s">
+      <c r="C9" s="3" t="s">
         <v>13</v>
       </c>
       <c r="G9" s="3"/>
@@ -703,8 +707,8 @@
       <c r="B10" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="F10" s="3" t="s">
-        <v>13</v>
+      <c r="F10" s="6" t="s">
+        <v>44</v>
       </c>
       <c r="G10" s="3" t="s">
         <v>18</v>

</xml_diff>